<commit_message>
updated design on wash performance
</commit_message>
<xml_diff>
--- a/NI-2010/Lab Drawings/AP1/Wash Performance/AP1 DOE BOM.xlsx
+++ b/NI-2010/Lab Drawings/AP1/Wash Performance/AP1 DOE BOM.xlsx
@@ -599,9 +599,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -653,6 +650,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -999,7 +999,7 @@
   <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H45" sqref="A1:H45"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,16 +1043,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1125,7 +1125,7 @@
         <v>62.2</v>
       </c>
       <c r="G4" s="12">
-        <f t="shared" ref="G4:G32" si="0">F4*B4</f>
+        <f t="shared" ref="G4:G30" si="0">F4*B4</f>
         <v>62.2</v>
       </c>
       <c r="H4" s="10" t="s">
@@ -1137,7 +1137,7 @@
       <c r="B5" s="7">
         <v>1</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="27" t="s">
         <v>121</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1162,7 +1162,7 @@
       <c r="B6" s="7">
         <v>1</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="27" t="s">
         <v>124</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -1267,19 +1267,19 @@
       <c r="A10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="28">
         <v>2</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="31">
+      <c r="F10" s="30">
         <v>390</v>
       </c>
       <c r="G10" s="12">
@@ -1294,19 +1294,19 @@
       <c r="A11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="28">
         <v>2</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="31">
+      <c r="F11" s="30">
         <v>390</v>
       </c>
       <c r="G11" s="12">
@@ -1567,7 +1567,7 @@
       <c r="B21" s="7">
         <v>1</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="27" t="s">
         <v>93</v>
       </c>
       <c r="D21" s="7" t="s">
@@ -1825,41 +1825,41 @@
       </c>
     </row>
     <row r="31" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
-      <c r="B31" s="34">
+      <c r="A31" s="31"/>
+      <c r="B31" s="33">
         <v>3</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="D31" s="34" t="s">
+      <c r="D31" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
       <c r="H31" s="10" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
-      <c r="B32" s="34">
+      <c r="A32" s="31"/>
+      <c r="B32" s="33">
         <v>2</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="D32" s="34" t="s">
+      <c r="D32" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="E32" s="32" t="s">
+      <c r="E32" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
       <c r="H32" s="10" t="s">
         <v>127</v>
       </c>
@@ -1890,7 +1890,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
+      <c r="A34" s="31"/>
       <c r="B34" s="7">
         <v>1</v>
       </c>
@@ -2169,180 +2169,180 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
-      <c r="B45" s="36" t="s">
+      <c r="A45" s="34"/>
+      <c r="B45" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36" t="s">
+      <c r="C45" s="35"/>
+      <c r="D45" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="E45" s="37" t="s">
+      <c r="E45" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="F45" s="38"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="35"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
+      <c r="A46" s="18"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="19"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="22"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
+      <c r="A47" s="18"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="27"/>
-      <c r="H48" s="27"/>
+      <c r="A48" s="22"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="27"/>
-      <c r="H49" s="27"/>
+      <c r="A49" s="22"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="24"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="24"/>
-      <c r="H50" s="27"/>
+      <c r="A50" s="23"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="23"/>
+      <c r="H50" s="26"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="19"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="22"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
+      <c r="A51" s="18"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="19"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="22"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
+      <c r="A52" s="18"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="19"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="22"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="20"/>
+      <c r="A53" s="18"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="19"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="22"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
+      <c r="A54" s="18"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="24"/>
-      <c r="B55" s="24"/>
-      <c r="C55" s="24"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="26"/>
-      <c r="G55" s="24"/>
-      <c r="H55" s="27"/>
+      <c r="A55" s="23"/>
+      <c r="B55" s="23"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="23"/>
+      <c r="H55" s="26"/>
     </row>
     <row r="56" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="18"/>
-      <c r="B56" s="33"/>
-      <c r="C56" s="33"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
+      <c r="A56" s="17"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
     </row>
     <row r="57" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="18"/>
-      <c r="B57" s="33"/>
-      <c r="C57" s="33"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
-      <c r="H57" s="18"/>
+      <c r="A57" s="17"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="24"/>
-      <c r="B58" s="24"/>
-      <c r="C58" s="24"/>
-      <c r="D58" s="24"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="26"/>
-      <c r="G58" s="24"/>
-      <c r="H58" s="27"/>
+      <c r="A58" s="23"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="26"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="19"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="20"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="21"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="20"/>
-      <c r="H59" s="20"/>
+      <c r="A59" s="18"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="19"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="24"/>
-      <c r="B60" s="24"/>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="26"/>
-      <c r="G60" s="27"/>
-      <c r="H60" s="27"/>
+      <c r="A60" s="23"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="25"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="26"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="24"/>
-      <c r="B61" s="24"/>
-      <c r="C61" s="24"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="26"/>
-      <c r="G61" s="27"/>
-      <c r="H61" s="27"/>
+      <c r="A61" s="23"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="25"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2364,16 +2364,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">

</xml_diff>